<commit_message>
Aspect bar for search SO Library
</commit_message>
<xml_diff>
--- a/database/Report Calculation.xlsx
+++ b/database/Report Calculation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dicha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\performance-tracking\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC78E2CF-C7D5-4101-A4A8-2C56AC8D9835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C76142-3929-460C-9168-206C37B47A3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{05208D3B-E17F-44B5-AAFE-C53CB084AF40}"/>
+    <workbookView xWindow="4596" yWindow="1836" windowWidth="17280" windowHeight="9072" xr2:uid="{05208D3B-E17F-44B5-AAFE-C53CB084AF40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>target</t>
   </si>
@@ -52,6 +52,24 @@
   </si>
   <si>
     <t>Perbandingan bulanan yang sama di tahun lalu</t>
+  </si>
+  <si>
+    <t>minimize</t>
+  </si>
+  <si>
+    <t>maximize</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>C tidak boleh 0</t>
   </si>
 </sst>
 </file>
@@ -415,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1C300F-BDCB-4F93-855A-975A21878B92}">
-  <dimension ref="A2:P27"/>
+  <dimension ref="A2:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -824,51 +842,51 @@
         <v>4</v>
       </c>
       <c r="C23">
-        <f>C16/C15</f>
+        <f t="shared" ref="C23:N23" si="0">C16/C15</f>
         <v>0.79</v>
       </c>
       <c r="D23">
-        <f>D16/D15</f>
+        <f t="shared" si="0"/>
         <v>0.34</v>
       </c>
       <c r="E23">
-        <f>E16/E15</f>
+        <f t="shared" si="0"/>
         <v>0.54</v>
       </c>
       <c r="F23">
-        <f>F16/F15</f>
+        <f t="shared" si="0"/>
         <v>0.45</v>
       </c>
       <c r="G23">
-        <f>G16/G15</f>
+        <f t="shared" si="0"/>
         <v>0.64</v>
       </c>
       <c r="H23">
-        <f>H16/H15</f>
+        <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
       <c r="I23">
-        <f>I16/I15</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J23">
-        <f>J16/J15</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="K23">
-        <f>K16/K15</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="L23">
-        <f>L16/L15</f>
+        <f t="shared" si="0"/>
         <v>0.79</v>
       </c>
       <c r="M23">
-        <f>M16/M15</f>
+        <f t="shared" si="0"/>
         <v>0.8</v>
       </c>
       <c r="N23">
-        <f>N16/N15</f>
+        <f t="shared" si="0"/>
         <v>0.88</v>
       </c>
     </row>
@@ -908,51 +926,51 @@
         <v>6</v>
       </c>
       <c r="C26">
-        <f>C16/C11</f>
+        <f t="shared" ref="C26:N26" si="1">C16/C11</f>
         <v>0.39500000000000002</v>
       </c>
       <c r="D26">
-        <f>D16/D11</f>
+        <f t="shared" si="1"/>
         <v>0.42499999999999999</v>
       </c>
       <c r="E26">
-        <f>E16/E11</f>
+        <f t="shared" si="1"/>
         <v>0.18</v>
       </c>
       <c r="F26">
-        <f>F16/F11</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="G26">
-        <f>G16/G11</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H26">
-        <f>H16/H11</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I26">
-        <f>I16/I11</f>
+        <f t="shared" si="1"/>
         <v>4.7619047619047619</v>
       </c>
       <c r="J26">
-        <f>J16/J11</f>
+        <f t="shared" si="1"/>
         <v>1.4814814814814814</v>
       </c>
       <c r="K26">
-        <f>K16/K11</f>
+        <f t="shared" si="1"/>
         <v>13.043478260869565</v>
       </c>
       <c r="L26">
-        <f>L16/L11</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M26">
-        <f>M16/M11</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="N26">
-        <f>N16/N11</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P26" t="s">
@@ -1010,6 +1028,52 @@
       <c r="N27">
         <f>SUM(C16:N16)/SUM(C15:N15)</f>
         <v>0.95750000000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>10.5</v>
+      </c>
+      <c r="D32">
+        <v>20</v>
+      </c>
+      <c r="E32">
+        <f>(C32/D32)*100</f>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>11</v>
+      </c>
+      <c r="E33">
+        <f>(D33/C33)*100</f>
+        <v>110.00000000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="D36" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revisi bug add custom kpi
</commit_message>
<xml_diff>
--- a/database/Report Calculation.xlsx
+++ b/database/Report Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\performance-tracking\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E14CD3DA-FA30-4755-834F-6029C16FF542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44B905E-44FD-41D6-A4F8-CDADB6AA838B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{05208D3B-E17F-44B5-AAFE-C53CB084AF40}"/>
   </bookViews>
@@ -175,13 +175,13 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1150,7 +1150,7 @@
   <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1161,23 +1161,23 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="4" t="s">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="4"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -1223,7 +1223,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>0.25</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -1232,29 +1232,29 @@
       <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>80</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>80</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="5">
         <v>70</v>
       </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6">
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5">
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>0.25</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -1265,23 +1265,23 @@
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <v>80</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="6"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
-      <c r="L7" s="6"/>
+      <c r="L7" s="5"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
-      <c r="O7" s="6">
+      <c r="O7" s="5">
         <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>0.25</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -1293,20 +1293,20 @@
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="6"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="6"/>
+      <c r="K8" s="5"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="6">
+      <c r="O8" s="5">
         <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="A9" s="4">
         <v>0.25</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1320,13 +1320,13 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="6"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
-      <c r="O9" s="6">
+      <c r="O9" s="5">
         <v>50</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update migration + initial personnel progress
</commit_message>
<xml_diff>
--- a/database/Report Calculation.xlsx
+++ b/database/Report Calculation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\performance-tracking\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979BB5D6-D893-4F26-A7A6-3D27346AEE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4B8700-794C-44F8-98D8-BA4689D179AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{05208D3B-E17F-44B5-AAFE-C53CB084AF40}"/>
   </bookViews>
@@ -499,7 +499,7 @@
   <dimension ref="A2:P36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
pembenaran db weighted score
</commit_message>
<xml_diff>
--- a/database/Report Calculation.xlsx
+++ b/database/Report Calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\performance-tracking\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4B8700-794C-44F8-98D8-BA4689D179AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F353B4-6F18-474D-A5B8-D53C1A00EA21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{05208D3B-E17F-44B5-AAFE-C53CB084AF40}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{05208D3B-E17F-44B5-AAFE-C53CB084AF40}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,7 +498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A1C300F-BDCB-4F93-855A-975A21878B92}">
   <dimension ref="A2:P36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C493CA92-4DE2-47F6-B7B2-586C99A2A9A9}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1255,7 +1255,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>17</v>
@@ -1282,7 +1282,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>18</v>
@@ -1358,7 +1358,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3">
         <f>F7*A7</f>
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -1370,7 +1370,7 @@
       <c r="N14" s="3"/>
       <c r="O14" s="3">
         <f t="shared" ref="O14:O16" si="0">O7*A7</f>
-        <v>17.5</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -1387,7 +1387,7 @@
       <c r="N15" s="3"/>
       <c r="O15" s="3">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -1413,12 +1413,12 @@
         <v>80</v>
       </c>
       <c r="F17">
-        <f>SUM(F13:F16)/50%</f>
-        <v>75</v>
+        <f>SUM(F13:F16)/SUM(A6:A7)</f>
+        <v>73.75</v>
       </c>
       <c r="O17">
         <f>SUM(O13:O16)/100%</f>
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>